<commit_message>
chore: update News.xlsx with new Moore-Czech releases
</commit_message>
<xml_diff>
--- a/News.xlsx
+++ b/News.xlsx
@@ -1,80 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ts174\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D99A184-B19F-426B-AC97-58F76E5E7836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{594E6574-2716-4346-AB20-ACE62EC5C43B}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Title Original</t>
-  </si>
-  <si>
-    <t>Content Original</t>
-  </si>
-  <si>
-    <t>Title ENG</t>
-  </si>
-  <si>
-    <t>Summary ENG</t>
-  </si>
-  <si>
-    <t>PostDate</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -93,35 +46,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9C51D73-345B-4069-9149-A8F403CED273}" name="News" displayName="News" ref="C3:I4" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="C3:I4" xr:uid="{D9C51D73-345B-4069-9149-A8F403CED273}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="News" displayName="News" ref="C3:I4" headerRowCount="1" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="C3:I4"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{5C9D83CE-F1FE-46A8-9230-284DBD1D365E}" name="Title Original"/>
-    <tableColumn id="2" xr3:uid="{4A95781C-F37D-4444-B646-8AAE2A11217D}" name="Content Original"/>
-    <tableColumn id="3" xr3:uid="{1D842EFB-A38D-4EEB-B02F-181B37242AC4}" name="Title ENG"/>
-    <tableColumn id="4" xr3:uid="{D2F7D12E-81CF-4896-BF8D-80CD7485044C}" name="Summary ENG"/>
-    <tableColumn id="5" xr3:uid="{E1BFB0E0-5932-4FF2-8488-594E25C3C335}" name="PostDate"/>
-    <tableColumn id="6" xr3:uid="{938A0573-96E4-4935-A057-2C7C4046D43C}" name="URL"/>
-    <tableColumn id="7" xr3:uid="{D6EAE848-EE71-4404-8EED-AAB1C31ECA58}" name="Source"/>
+    <tableColumn id="1" name="Title Original"/>
+    <tableColumn id="2" name="Content Original"/>
+    <tableColumn id="3" name="Title ENG"/>
+    <tableColumn id="4" name="Summary ENG"/>
+    <tableColumn id="5" name="PostDate"/>
+    <tableColumn id="6" name="URL"/>
+    <tableColumn id="7" name="Source"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -443,50 +455,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B6242B-943C-4733-ADFC-397F3DA6C618}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="C3:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.33203125" customWidth="1"/>
+    <col width="13.77734375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="16.77734375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.109375" customWidth="1" min="5" max="5"/>
+    <col width="15.33203125" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="10.77734375" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="10.33203125" customWidth="1" min="8" max="10"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>6</v>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Title Original</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Content Original</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Title ENG</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Summary ENG</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>PostDate</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>